<commit_message>
#1: cập nhật tài liệu Lesson1.xlsx
</commit_message>
<xml_diff>
--- a/0.Document/Training/Lesson1.xlsx
+++ b/0.Document/Training/Lesson1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Vị trí nằm giữa màn hình cách lề trên 200px</t>
   </si>
@@ -49,6 +49,18 @@
   </si>
   <si>
     <t xml:space="preserve">Push trên branch mới theo format: </t>
+  </si>
+  <si>
+    <t>Comment khi push</t>
+  </si>
+  <si>
+    <t>#{số issue}: comment</t>
+  </si>
+  <si>
+    <t>#1: hoàn thành lesson 1</t>
+  </si>
+  <si>
+    <t>vd: Khi hoàn thành lesson 1 ở https://github.com/VHEC-NAMTT/asp_net_training/issues/1 khi push sẽ ghi</t>
   </si>
 </sst>
 </file>
@@ -415,15 +427,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="3" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="4" style="1"/>
-    <col min="4" max="4" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="4" style="1"/>
+    <col min="1" max="16384" width="3" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -443,10 +453,9 @@
         <v>9</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="4">
+      <c r="E2" s="4">
         <v>1</v>
       </c>
-      <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -492,7 +501,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>8</v>
       </c>
@@ -505,7 +514,7 @@
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
       <c r="C19" s="5" t="s">
         <v>10</v>
@@ -518,11 +527,11 @@
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5" t="str">
-        <f>"Lesson-"&amp;D2&amp;"-{tên user}"</f>
+        <f>"Lesson-"&amp;E2&amp;"-{tên user}"</f>
         <v>Lesson-1-{tên user}</v>
       </c>
       <c r="E20" s="5"/>
@@ -532,19 +541,74 @@
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
-      <c r="C21" s="5" t="str">
-        <f>"vd: Lesson-"&amp;D2&amp;"-an"</f>
+      <c r="D21" s="5" t="str">
+        <f>"vd: Lesson-"&amp;E2&amp;"-an"</f>
         <v>vd: Lesson-1-an</v>
       </c>
-      <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C23" s="5"/>
+      <c r="D23" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C24" s="5"/>
+      <c r="D24" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -556,7 +620,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>